<commit_message>
Getting total winnings working
</commit_message>
<xml_diff>
--- a/fg/external_files/tournaments.xlsx
+++ b/fg/external_files/tournaments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexevans/Library/Containers/com.microsoft.Excel/Data/Desktop/Projects/fgolf/fg/external_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2489DF-F856-C944-87CD-BE0B3C7DA949}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD4450A-FFCC-544F-AB3F-1196B850EEAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="1440" windowWidth="27200" windowHeight="14900" xr2:uid="{30A812C3-CDC1-F54E-A767-28DF1283A54D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>TOURNAMENT</t>
   </si>
@@ -187,6 +187,45 @@
   </si>
   <si>
     <t>2019-08-25</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056547</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056527</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard/_/tournamentId/401056550</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056551</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056552</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056554</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056556</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056558</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056548</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056544</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056543</t>
+  </si>
+  <si>
+    <t>https://www.espn.com/golf/leaderboard?tournamentId=401056542</t>
   </si>
 </sst>
 </file>
@@ -545,16 +584,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FDA558-F8D1-BE44-BE78-45A62A23DC89}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +608,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -581,8 +625,11 @@
       <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -595,8 +642,11 @@
       <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -609,8 +659,11 @@
       <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -623,8 +676,11 @@
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -637,8 +693,11 @@
       <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -651,8 +710,11 @@
       <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -665,8 +727,11 @@
       <c r="D8" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -679,8 +744,11 @@
       <c r="D9" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -693,8 +761,11 @@
       <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -707,8 +778,11 @@
       <c r="D11" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -721,8 +795,11 @@
       <c r="D12" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -734,6 +811,9 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>